<commit_message>
single particle bug fix, signle camera combobox bug fix, report change radius to diamerer
</commit_message>
<xml_diff>
--- a/calculations doc/fps calc.xlsx
+++ b/calculations doc/fps calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amir\Desktop\Paticle_Size_Analyser\calculations doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20CDFFF-82E7-492B-91C6-BCBF2A8DF54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2C8C26-1528-48C6-9DBD-D98549189624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AA7F440D-F57D-49DC-A5EF-0213552AADA9}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I21" sqref="I21:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,34 +432,34 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>9.8000000000000007</v>
       </c>
       <c r="C2">
         <f>A2/1000</f>
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D2">
         <f>SQRT(C2*2/B2)*1000</f>
-        <v>110.65666703449763</v>
+        <v>115.17511068997928</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B3">
         <v>9.8000000000000007</v>
       </c>
       <c r="C3">
         <f>A3/1000</f>
-        <v>0.16</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D3">
         <f>SQRT(C3*2/B3)*1000</f>
-        <v>180.70158058105022</v>
+        <v>169.03085094570329</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -473,11 +473,11 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D6">
         <f>D3-D2</f>
-        <v>70.044913546552593</v>
+        <v>53.855740255724015</v>
       </c>
       <c r="E6">
         <f>1000/D6</f>
-        <v>14.276554133161852</v>
+        <v>18.568122826864602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>